<commit_message>
Added WateringSettingsMenu and ResetMenu (not tested)
</commit_message>
<xml_diff>
--- a/watering1/memory.xlsx
+++ b/watering1/memory.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>halk</t>
   </si>
@@ -81,9 +81,6 @@
     <t>backlightMode</t>
   </si>
   <si>
-    <t>cumulativeHour</t>
-  </si>
-  <si>
     <t>hourOfDay</t>
   </si>
   <si>
@@ -91,6 +88,12 @@
   </si>
   <si>
     <t>wateringStatus</t>
+  </si>
+  <si>
+    <t>wateringRecordIndex</t>
+  </si>
+  <si>
+    <t>cumulativeRunningHour</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D27"/>
+  <dimension ref="A2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +459,7 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -468,7 +471,7 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+B2*C3</f>
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -484,7 +487,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+C4*B7</f>
-        <v>626</v>
+        <v>636</v>
       </c>
       <c r="B4">
         <v>24</v>
@@ -500,7 +503,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4+B8*C5</f>
-        <v>866</v>
+        <v>876</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -542,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -551,7 +554,7 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>A17+B17</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -562,35 +565,35 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" ref="A19:A27" si="0">A18+B18</f>
-        <v>2</v>
+        <f>A18+B18</f>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" ref="A20:A28" si="0">A19+B19</f>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
@@ -599,10 +602,10 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B22">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
@@ -611,37 +614,49 @@
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B23">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>55</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First version of automatic watering
</commit_message>
<xml_diff>
--- a/watering1/memory.xlsx
+++ b/watering1/memory.xlsx
@@ -449,7 +449,7 @@
   <dimension ref="A2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,14 +503,14 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4+B8*C5</f>
-        <v>876</v>
+        <v>906</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
       <c r="C5">
         <f>B5*B9</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -537,7 +537,7 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>